<commit_message>
current status of cloud 11/11/2024
</commit_message>
<xml_diff>
--- a/public/export_with_letterhead.xlsx
+++ b/public/export_with_letterhead.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>School ID</t>
   </si>
@@ -44,7 +44,7 @@
     <t>Date Added</t>
   </si>
   <si>
-    <t>Malinta National High School</t>
+    <t>Global Reciprocal College</t>
   </si>
   <si>
     <t>public</t>
@@ -56,55 +56,46 @@
     <t>Congressional I</t>
   </si>
   <si>
-    <t>MNHS Admin</t>
-  </si>
-  <si>
-    <t>09123456789</t>
-  </si>
-  <si>
-    <t>xandrexxenosaquinde@gmail.com</t>
-  </si>
-  <si>
-    <t>2024-09-03 23:52:39</t>
-  </si>
-  <si>
-    <t>West National High School</t>
+    <t>grc</t>
+  </si>
+  <si>
+    <t>08745120956230</t>
+  </si>
+  <si>
+    <t>grc@gmail.com</t>
+  </si>
+  <si>
+    <t>2024-10-24 08:26:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grc@gmail.com	</t>
+  </si>
+  <si>
+    <t>2024-10-24 10:22:51</t>
+  </si>
+  <si>
+    <t>ELI School</t>
   </si>
   <si>
     <t>private</t>
   </si>
   <si>
-    <t>Lorem Ipsum</t>
+    <t>2024-10-25 10:46:59</t>
+  </si>
+  <si>
+    <t>Maysan National High School</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum A</t>
   </si>
   <si>
     <t>09060158736</t>
   </si>
   <si>
-    <t>123@1.com</t>
-  </si>
-  <si>
-    <t>2024-09-04 01:25:53</t>
-  </si>
-  <si>
-    <t>Dalandanan National High School</t>
-  </si>
-  <si>
-    <t>2024-09-04 01:48:42</t>
-  </si>
-  <si>
-    <t>Maysan National High School</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum A</t>
+    <t>exonatural321@gmail.com</t>
   </si>
   <si>
     <t>2024-09-04 01:50:22</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>2024-09-15 10:39:24</t>
   </si>
 </sst>
 </file>
@@ -479,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +510,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>111222</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -548,13 +539,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>222444</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -563,27 +554,27 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>9123456893</v>
       </c>
       <c r="H9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>333444</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -591,17 +582,8 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
-      <c r="F10">
-        <v>12345</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -609,7 +591,7 @@
         <v>555666</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -621,45 +603,16 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>999999</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12">
-        <v>12345</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scrollable Filter and Export PDF
</commit_message>
<xml_diff>
--- a/public/export_with_letterhead.xlsx
+++ b/public/export_with_letterhead.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
   <si>
     <t>School ID</t>
   </si>
@@ -68,10 +68,7 @@
     <t>2024-09-03 23:52:39</t>
   </si>
   <si>
-    <t>West National High School</t>
-  </si>
-  <si>
-    <t>private</t>
+    <t>Canumay West National High School</t>
   </si>
   <si>
     <t>Lorem Ipsum</t>
@@ -554,7 +551,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -563,16 +560,16 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -580,7 +577,7 @@
         <v>333444</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
@@ -595,13 +592,13 @@
         <v>12345</v>
       </c>
       <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
         <v>20</v>
       </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -609,7 +606,7 @@
         <v>555666</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -621,16 +618,16 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" t="s">
         <v>26</v>
-      </c>
-      <c r="G11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -638,7 +635,7 @@
         <v>999999</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
@@ -653,13 +650,13 @@
         <v>12345</v>
       </c>
       <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
         <v>20</v>
       </c>
-      <c r="H12" t="s">
-        <v>21</v>
-      </c>
       <c r="I12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>